<commit_message>
Added Assignment 3 to WBA
</commit_message>
<xml_diff>
--- a/WBA.xlsx
+++ b/WBA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariehendrikse/Documents/UNITS/FIT2099/Project 1/Untitled.py/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://monashuni-my.sharepoint.com/personal/rsta0012_student_monash_edu/Documents/Uni Stuff/Semester 1 - 2020/FIT2099/Assignment/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150947BF-1754-4D4A-83D2-08FEDBB3F15E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="114_{7187AB2F-1C1F-408C-8B77-7A5306A30756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2E661D27-4E02-4C96-820A-50179AAF8279}"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="2120" windowWidth="22700" windowHeight="14600" xr2:uid="{8D13EC75-E73C-4807-BBD1-A91D9A88616D}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11250" xr2:uid="{8D13EC75-E73C-4807-BBD1-A91D9A88616D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
   <si>
     <t>Task</t>
   </si>
@@ -87,6 +87,30 @@
   </si>
   <si>
     <t>Implementation Plan and Documentation (Due 8th of May)</t>
+  </si>
+  <si>
+    <t>Going to Town</t>
+  </si>
+  <si>
+    <t>Mambo Marie</t>
+  </si>
+  <si>
+    <t>Ending the Game</t>
+  </si>
+  <si>
+    <t>Guns</t>
+  </si>
+  <si>
+    <t>8th of June</t>
+  </si>
+  <si>
+    <t>Code and Documentation Have Ready By</t>
+  </si>
+  <si>
+    <t>Recommendations Report</t>
+  </si>
+  <si>
+    <t>Both (Half/Half)</t>
   </si>
 </sst>
 </file>
@@ -146,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -158,6 +182,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -181,15 +217,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>204788</xdr:colOff>
+      <xdr:colOff>585789</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>252413</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>61913</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -204,8 +240,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5891213" y="180974"/>
-          <a:ext cx="3286125" cy="1871664"/>
+          <a:off x="5938839" y="190499"/>
+          <a:ext cx="2957512" cy="2095501"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -584,27 +620,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2C31CF-E103-4072-92F1-C16204AB2BD2}">
-  <dimension ref="B2:F8"/>
+  <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="2:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,7 +658,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -638,7 +675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -655,7 +692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -672,7 +709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -689,7 +726,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -706,9 +743,93 @@
         <v>15</v>
       </c>
     </row>
+    <row r="9" spans="2:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="7">
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -717,12 +838,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -949,15 +1067,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83978174-F81A-4541-AE42-BDFD5E09B1D7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DB619BC-C5BE-491A-B7A4-DC7310986F01}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="50d67897-3669-4ebb-befc-92a766fd0fcb"/>
+    <ds:schemaRef ds:uri="de9833e3-938e-4cc4-9ba0-60543af0dc30"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -982,18 +1112,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DB619BC-C5BE-491A-B7A4-DC7310986F01}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83978174-F81A-4541-AE42-BDFD5E09B1D7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="50d67897-3669-4ebb-befc-92a766fd0fcb"/>
-    <ds:schemaRef ds:uri="de9833e3-938e-4cc4-9ba0-60543af0dc30"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added further explanation to the 'Going to Town' design rationale
</commit_message>
<xml_diff>
--- a/WBA.xlsx
+++ b/WBA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://monashuni-my.sharepoint.com/personal/rsta0012_student_monash_edu/Documents/Uni Stuff/Semester 1 - 2020/FIT2099/Assignment/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="114_{7187AB2F-1C1F-408C-8B77-7A5306A30756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2E661D27-4E02-4C96-820A-50179AAF8279}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="114_{7187AB2F-1C1F-408C-8B77-7A5306A30756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9000D4E4-1F03-447F-99C8-68B759E29F6B}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11250" xr2:uid="{8D13EC75-E73C-4807-BBD1-A91D9A88616D}"/>
   </bookViews>
@@ -180,20 +180,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -623,7 +623,7 @@
   <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,10 +636,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -744,40 +744,40 @@
       </c>
     </row>
     <row r="9" spans="2:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
@@ -789,37 +789,37 @@
       <c r="D12" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -838,9 +838,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1067,27 +1070,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DB619BC-C5BE-491A-B7A4-DC7310986F01}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83978174-F81A-4541-AE42-BDFD5E09B1D7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="50d67897-3669-4ebb-befc-92a766fd0fcb"/>
-    <ds:schemaRef ds:uri="de9833e3-938e-4cc4-9ba0-60543af0dc30"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1112,9 +1103,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83978174-F81A-4541-AE42-BDFD5E09B1D7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DB619BC-C5BE-491A-B7A4-DC7310986F01}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="50d67897-3669-4ebb-befc-92a766fd0fcb"/>
+    <ds:schemaRef ds:uri="de9833e3-938e-4cc4-9ba0-60543af0dc30"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>